<commit_message>
imf data on USA, uk and China added
</commit_message>
<xml_diff>
--- a/notebooks/imf_rawdata/imf_debt.xlsx
+++ b/notebooks/imf_rawdata/imf_debt.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -520,10 +520,10 @@
     <t xml:space="preserve">Ukraine</t>
   </si>
   <si>
-    <t xml:space="preserve">United Kingdom</t>
+    <t xml:space="preserve">United Kingdom of Great Britain and Northern Ireland</t>
   </si>
   <si>
-    <t xml:space="preserve">United States</t>
+    <t xml:space="preserve">United States of America</t>
   </si>
   <si>
     <t xml:space="preserve">Uruguay</t>
@@ -566,6 +566,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -653,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:BS178"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>